<commit_message>
melhoria de varios setores
</commit_message>
<xml_diff>
--- a/Projects/CompanyManagement/Products.xlsx
+++ b/Projects/CompanyManagement/Products.xlsx
@@ -1,16 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\march\OneDrive\Documentos\Projects\DataScience\Projects\CompanyManagement\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AD46668-36E2-4035-86DC-C7B39281285E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="CustosVariaveis" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="CustosFixos" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Pratos" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="CustosExtras" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="Vendas" sheetId="5" r:id="rId8"/>
+    <sheet name="CustosVariaveis" sheetId="1" r:id="rId1"/>
+    <sheet name="CustosFixos" sheetId="2" r:id="rId2"/>
+    <sheet name="Pratos" sheetId="3" r:id="rId3"/>
+    <sheet name="CustosExtras" sheetId="4" r:id="rId4"/>
+    <sheet name="Vendas" sheetId="5" r:id="rId5"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -248,25 +257,26 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
-    <numFmt numFmtId="165" formatCode="hh:mm"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -277,67 +287,50 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="20" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -527,25 +520,28 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="21.25"/>
-    <col customWidth="1" min="3" max="3" width="15.88"/>
-    <col customWidth="1" min="4" max="4" width="13.75"/>
+    <col min="2" max="2" width="21.21875" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -559,320 +555,321 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="2">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="2">
-        <v>300.0</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="2">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="2">
-        <v>60.0</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="2">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="2">
-        <v>45.0</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="2">
-        <v>80.0</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="2">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="2">
-        <v>120.0</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="2">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="2">
-        <v>30.0</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="2">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="2">
-        <v>50.0</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D9" s="2">
-        <v>100.0</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="2">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D10" s="2">
-        <v>240.0</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="2">
-        <v>28.0</v>
+        <v>28</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D11" s="2">
-        <v>128.0</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B12" s="2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D12" s="2">
-        <v>90.0</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B13" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D13" s="2">
-        <v>75.0</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D14" s="2">
-        <v>200.0</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="2">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D15" s="2">
-        <v>45.0</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B16" s="2">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D16" s="2">
-        <v>96.0</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B17" s="2">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="2">
-        <v>150.0</v>
-      </c>
-    </row>
-    <row r="18">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B18" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="2">
-        <v>90.0</v>
-      </c>
-    </row>
-    <row r="19">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B19" s="2">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D19" s="2">
-        <v>50.0</v>
-      </c>
-    </row>
-    <row r="20">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B20" s="2">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D20" s="2">
-        <v>30.0</v>
-      </c>
-    </row>
-    <row r="21">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B21" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D21" s="2">
-        <v>70.0</v>
-      </c>
-    </row>
-    <row r="22">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B22" s="2">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D22" s="2">
-        <v>28.0</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="38.25"/>
-    <col customWidth="1" min="2" max="2" width="15.0"/>
+    <col min="1" max="1" width="38.21875" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
@@ -880,130 +877,133 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B2" s="4">
-        <v>2000.0</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B3" s="4">
-        <v>4000.0</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B4" s="2">
-        <v>100.0</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B5" s="4">
-        <v>800.0</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B6" s="2">
-        <v>400.0</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B7" s="2">
-        <v>100.0</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B8" s="2">
-        <v>200.0</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B9" s="2">
-        <v>600.0</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B10" s="2">
-        <v>300.0</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B11" s="4">
-        <v>50.0</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B12" s="2">
-        <v>700.0</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B13" s="4">
-        <v>500.0</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B14" s="2">
-        <v>200.0</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="18.38"/>
-    <col customWidth="1" min="2" max="2" width="295.13"/>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="295.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>43</v>
       </c>
@@ -1011,7 +1011,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>45</v>
       </c>
@@ -1019,7 +1019,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>47</v>
       </c>
@@ -1027,7 +1027,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>49</v>
       </c>
@@ -1035,7 +1035,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>51</v>
       </c>
@@ -1043,7 +1043,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>53</v>
       </c>
@@ -1051,7 +1051,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>55</v>
       </c>
@@ -1059,7 +1059,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>57</v>
       </c>
@@ -1067,7 +1067,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>59</v>
       </c>
@@ -1075,7 +1075,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>61</v>
       </c>
@@ -1083,7 +1083,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>63</v>
       </c>
@@ -1091,7 +1091,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>65</v>
       </c>
@@ -1099,7 +1099,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>67</v>
       </c>
@@ -1107,7 +1107,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>69</v>
       </c>
@@ -1116,26 +1116,27 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="18.38"/>
-    <col customWidth="1" min="2" max="2" width="17.63"/>
-    <col customWidth="1" min="3" max="3" width="15.13"/>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>43</v>
       </c>
@@ -1146,311 +1147,317 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B2" s="2">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="C2" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B3" s="2">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="C3" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B4" s="2">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="C4" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B5" s="2">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="C5" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B6" s="2">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="C6" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B7" s="2">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="C7" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B8" s="2">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="C8" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B9" s="2">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="C9" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>61</v>
       </c>
       <c r="B10" s="2">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="C10" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B11" s="2">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="C11" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>65</v>
       </c>
       <c r="B12" s="2">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="C12" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>67</v>
       </c>
       <c r="B13" s="2">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="C13" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>69</v>
       </c>
       <c r="B14" s="2">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="C14" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B15" s="2">
-        <v>300.0</v>
+        <v>300</v>
       </c>
       <c r="C15" s="2">
-        <v>1000.0</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B16" s="2">
-        <v>300.0</v>
+        <v>300</v>
       </c>
       <c r="C16" s="2">
-        <v>300.0</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B17" s="2">
-        <v>300.0</v>
+        <v>300</v>
       </c>
       <c r="C17" s="2">
-        <v>400.0</v>
-      </c>
-    </row>
-    <row r="18">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B18" s="2">
-        <v>300.0</v>
+        <v>300</v>
       </c>
       <c r="C18" s="2">
-        <v>6000.0</v>
-      </c>
-    </row>
-    <row r="19">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B19" s="2">
-        <v>300.0</v>
+        <v>300</v>
       </c>
       <c r="C19" s="2">
-        <v>23.0</v>
-      </c>
-    </row>
-    <row r="20">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B20" s="2">
-        <v>300.0</v>
+        <v>300</v>
       </c>
       <c r="C20" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B21" s="2">
-        <v>300.0</v>
+        <v>300</v>
       </c>
       <c r="C21" s="2">
-        <v>245.0</v>
-      </c>
-    </row>
-    <row r="22">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B22" s="2">
-        <v>300.0</v>
+        <v>300</v>
       </c>
       <c r="C22" s="2">
-        <v>2345.0</v>
-      </c>
-    </row>
-    <row r="23">
+        <v>2345</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>61</v>
       </c>
       <c r="B23" s="2">
-        <v>300.0</v>
+        <v>300</v>
       </c>
       <c r="C23" s="2">
-        <v>23123.0</v>
-      </c>
-    </row>
-    <row r="24">
+        <v>23123</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B24" s="2">
-        <v>300.0</v>
+        <v>300</v>
       </c>
       <c r="C24" s="2">
-        <v>543.0</v>
-      </c>
-    </row>
-    <row r="25">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>65</v>
       </c>
       <c r="B25" s="2">
-        <v>300.0</v>
+        <v>300</v>
       </c>
       <c r="C25" s="2">
-        <v>32432.0</v>
-      </c>
-    </row>
-    <row r="26">
+        <v>32432</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>67</v>
       </c>
       <c r="B26" s="2">
-        <v>300.0</v>
+        <v>300</v>
       </c>
       <c r="C26" s="2">
-        <v>323.0</v>
-      </c>
-    </row>
-    <row r="27">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>69</v>
       </c>
       <c r="B27" s="2">
-        <v>300.0</v>
+        <v>300</v>
       </c>
       <c r="C27" s="2">
-        <v>43223.0</v>
+        <v>43223</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:D111"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="16.38"/>
+    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>43</v>
       </c>
@@ -1464,1547 +1471,1547 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B2" s="2">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="C2" s="5">
-        <v>45294.0</v>
+        <v>45294</v>
       </c>
       <c r="D2" s="6">
-        <v>0.7916666666666666</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>0.79166666666666663</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B3" s="2">
-        <v>28.0</v>
+        <v>28</v>
       </c>
       <c r="C3" s="5">
-        <v>45294.0</v>
+        <v>45294</v>
       </c>
       <c r="D3" s="6">
         <v>0.8125</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B4" s="2">
-        <v>28.0</v>
+        <v>28</v>
       </c>
       <c r="C4" s="5">
-        <v>45294.0</v>
+        <v>45294</v>
       </c>
       <c r="D4" s="6">
-        <v>0.8229166666666666</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>0.82291666666666663</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B5" s="2">
-        <v>40.0</v>
+        <v>40</v>
       </c>
       <c r="C5" s="5">
-        <v>45294.0</v>
+        <v>45294</v>
       </c>
       <c r="D5" s="6">
-        <v>0.8333333333333334</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B6" s="2">
-        <v>22.0</v>
+        <v>22</v>
       </c>
       <c r="C6" s="5">
-        <v>45294.0</v>
+        <v>45294</v>
       </c>
       <c r="D6" s="6">
         <v>0.84375</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>61</v>
       </c>
       <c r="B7" s="2">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="C7" s="5">
-        <v>45295.0</v>
+        <v>45295</v>
       </c>
       <c r="D7" s="6">
-        <v>0.5208333333333334</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>0.52083333333333337</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B8" s="2">
-        <v>32.0</v>
+        <v>32</v>
       </c>
       <c r="C8" s="5">
-        <v>45295.0</v>
+        <v>45295</v>
       </c>
       <c r="D8" s="6">
         <v>0.53125</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B9" s="2">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="C9" s="5">
-        <v>45295.0</v>
+        <v>45295</v>
       </c>
       <c r="D9" s="6">
-        <v>0.5416666666666666</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>0.54166666666666663</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B10" s="2">
-        <v>23.0</v>
+        <v>23</v>
       </c>
       <c r="C10" s="5">
-        <v>45295.0</v>
+        <v>45295</v>
       </c>
       <c r="D10" s="6">
-        <v>0.5520833333333334</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>0.55208333333333337</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B11" s="2">
-        <v>35.0</v>
+        <v>35</v>
       </c>
       <c r="C11" s="5">
-        <v>45295.0</v>
+        <v>45295</v>
       </c>
       <c r="D11" s="6">
-        <v>0.7708333333333334</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>0.77083333333333337</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B12" s="2">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="C12" s="5">
-        <v>45295.0</v>
+        <v>45295</v>
       </c>
       <c r="D12" s="6">
         <v>0.78125</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B13" s="2">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="C13" s="5">
-        <v>45296.0</v>
+        <v>45296</v>
       </c>
       <c r="D13" s="6">
-        <v>0.7916666666666666</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>0.79166666666666663</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B14" s="2">
-        <v>28.0</v>
+        <v>28</v>
       </c>
       <c r="C14" s="5">
-        <v>45296.0</v>
+        <v>45296</v>
       </c>
       <c r="D14" s="6">
-        <v>0.8020833333333334</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>0.80208333333333337</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B15" s="2">
-        <v>22.0</v>
+        <v>22</v>
       </c>
       <c r="C15" s="5">
-        <v>45296.0</v>
+        <v>45296</v>
       </c>
       <c r="D15" s="6">
         <v>0.8125</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B16" s="2">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="C16" s="5">
-        <v>45296.0</v>
+        <v>45296</v>
       </c>
       <c r="D16" s="6">
-        <v>0.8229166666666666</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>0.82291666666666663</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B17" s="2">
-        <v>29.0</v>
+        <v>29</v>
       </c>
       <c r="C17" s="5">
-        <v>45296.0</v>
+        <v>45296</v>
       </c>
       <c r="D17" s="6">
-        <v>0.8333333333333334</v>
-      </c>
-    </row>
-    <row r="18">
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>61</v>
       </c>
       <c r="B18" s="2">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="C18" s="5">
-        <v>45296.0</v>
+        <v>45296</v>
       </c>
       <c r="D18" s="6">
         <v>0.84375</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B19" s="2">
-        <v>42.0</v>
+        <v>42</v>
       </c>
       <c r="C19" s="5">
-        <v>45297.0</v>
+        <v>45297</v>
       </c>
       <c r="D19" s="6">
         <v>0.5</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>67</v>
       </c>
       <c r="B20" s="2">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="C20" s="5">
-        <v>45297.0</v>
+        <v>45297</v>
       </c>
       <c r="D20" s="6">
-        <v>0.5208333333333334</v>
-      </c>
-    </row>
-    <row r="21">
+        <v>0.52083333333333337</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B21" s="2">
-        <v>31.0</v>
+        <v>31</v>
       </c>
       <c r="C21" s="5">
-        <v>45297.0</v>
+        <v>45297</v>
       </c>
       <c r="D21" s="6">
         <v>0.53125</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B22" s="2">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="C22" s="5">
-        <v>45297.0</v>
+        <v>45297</v>
       </c>
       <c r="D22" s="6">
-        <v>0.5416666666666666</v>
-      </c>
-    </row>
-    <row r="23">
+        <v>0.54166666666666663</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B23" s="2">
-        <v>26.0</v>
+        <v>26</v>
       </c>
       <c r="C23" s="5">
-        <v>45297.0</v>
+        <v>45297</v>
       </c>
       <c r="D23" s="6">
-        <v>0.5520833333333334</v>
-      </c>
-    </row>
-    <row r="24">
+        <v>0.55208333333333337</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B24" s="2">
-        <v>23.0</v>
+        <v>23</v>
       </c>
       <c r="C24" s="5">
-        <v>45297.0</v>
+        <v>45297</v>
       </c>
       <c r="D24" s="6">
         <v>0.75</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B25" s="2">
-        <v>27.0</v>
+        <v>27</v>
       </c>
       <c r="C25" s="5">
-        <v>45297.0</v>
+        <v>45297</v>
       </c>
       <c r="D25" s="6">
-        <v>0.7604166666666666</v>
-      </c>
-    </row>
-    <row r="26">
+        <v>0.76041666666666663</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B26" s="2">
-        <v>38.0</v>
+        <v>38</v>
       </c>
       <c r="C26" s="5">
-        <v>45297.0</v>
+        <v>45297</v>
       </c>
       <c r="D26" s="6">
-        <v>0.7708333333333334</v>
-      </c>
-    </row>
-    <row r="27">
+        <v>0.77083333333333337</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B27" s="2">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="C27" s="5">
-        <v>45297.0</v>
+        <v>45297</v>
       </c>
       <c r="D27" s="6">
         <v>0.78125</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B28" s="2">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="C28" s="5">
-        <v>45297.0</v>
+        <v>45297</v>
       </c>
       <c r="D28" s="6">
-        <v>0.7916666666666666</v>
-      </c>
-    </row>
-    <row r="29">
+        <v>0.79166666666666663</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B29" s="2">
-        <v>27.0</v>
+        <v>27</v>
       </c>
       <c r="C29" s="5">
-        <v>45297.0</v>
+        <v>45297</v>
       </c>
       <c r="D29" s="6">
-        <v>0.8020833333333334</v>
-      </c>
-    </row>
-    <row r="30">
+        <v>0.80208333333333337</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>61</v>
       </c>
       <c r="B30" s="2">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="C30" s="5">
-        <v>45297.0</v>
+        <v>45297</v>
       </c>
       <c r="D30" s="6">
         <v>0.8125</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B31" s="2">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="C31" s="5">
-        <v>45294.0</v>
+        <v>45294</v>
       </c>
       <c r="D31" s="6">
-        <v>0.7916666666666666</v>
-      </c>
-    </row>
-    <row r="32">
+        <v>0.79166666666666663</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B32" s="2">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="C32" s="5">
-        <v>45294.0</v>
+        <v>45294</v>
       </c>
       <c r="D32" s="6">
-        <v>0.8020833333333334</v>
-      </c>
-    </row>
-    <row r="33">
+        <v>0.80208333333333337</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B33" s="2">
-        <v>28.0</v>
+        <v>28</v>
       </c>
       <c r="C33" s="5">
-        <v>45294.0</v>
+        <v>45294</v>
       </c>
       <c r="D33" s="6">
         <v>0.8125</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B34" s="2">
-        <v>28.0</v>
+        <v>28</v>
       </c>
       <c r="C34" s="5">
-        <v>45294.0</v>
+        <v>45294</v>
       </c>
       <c r="D34" s="6">
-        <v>0.8229166666666666</v>
-      </c>
-    </row>
-    <row r="35">
+        <v>0.82291666666666663</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B35" s="2">
-        <v>40.0</v>
+        <v>40</v>
       </c>
       <c r="C35" s="5">
-        <v>45294.0</v>
+        <v>45294</v>
       </c>
       <c r="D35" s="6">
-        <v>0.8333333333333334</v>
-      </c>
-    </row>
-    <row r="36">
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B36" s="2">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="C36" s="5">
-        <v>45294.0</v>
+        <v>45294</v>
       </c>
       <c r="D36" s="6">
         <v>0.84375</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>61</v>
       </c>
       <c r="B37" s="2">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="C37" s="5">
-        <v>45295.0</v>
+        <v>45295</v>
       </c>
       <c r="D37" s="6">
-        <v>0.5208333333333334</v>
-      </c>
-    </row>
-    <row r="38">
+        <v>0.52083333333333337</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B38" s="2">
-        <v>32.0</v>
+        <v>32</v>
       </c>
       <c r="C38" s="5">
-        <v>45295.0</v>
+        <v>45295</v>
       </c>
       <c r="D38" s="6">
         <v>0.53125</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B39" s="2">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="C39" s="5">
-        <v>45295.0</v>
+        <v>45295</v>
       </c>
       <c r="D39" s="6">
-        <v>0.5416666666666666</v>
-      </c>
-    </row>
-    <row r="40">
+        <v>0.54166666666666663</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B40" s="2">
-        <v>23.0</v>
+        <v>23</v>
       </c>
       <c r="C40" s="5">
-        <v>45295.0</v>
+        <v>45295</v>
       </c>
       <c r="D40" s="6">
-        <v>0.5520833333333334</v>
-      </c>
-    </row>
-    <row r="41">
+        <v>0.55208333333333337</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B41" s="2">
-        <v>35.0</v>
+        <v>35</v>
       </c>
       <c r="C41" s="5">
-        <v>45295.0</v>
+        <v>45295</v>
       </c>
       <c r="D41" s="6">
-        <v>0.7708333333333334</v>
-      </c>
-    </row>
-    <row r="42">
+        <v>0.77083333333333337</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B42" s="2">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="C42" s="5">
-        <v>45295.0</v>
+        <v>45295</v>
       </c>
       <c r="D42" s="6">
         <v>0.78125</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B43" s="2">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="C43" s="5">
-        <v>45296.0</v>
+        <v>45296</v>
       </c>
       <c r="D43" s="6">
-        <v>0.7916666666666666</v>
-      </c>
-    </row>
-    <row r="44">
+        <v>0.79166666666666663</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B44" s="2">
-        <v>28.0</v>
+        <v>28</v>
       </c>
       <c r="C44" s="5">
-        <v>45296.0</v>
+        <v>45296</v>
       </c>
       <c r="D44" s="6">
-        <v>0.8020833333333334</v>
-      </c>
-    </row>
-    <row r="45">
+        <v>0.80208333333333337</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B45" s="2">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="C45" s="5">
-        <v>45296.0</v>
+        <v>45296</v>
       </c>
       <c r="D45" s="6">
-        <v>0.8229166666666666</v>
-      </c>
-    </row>
-    <row r="46">
+        <v>0.82291666666666663</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B46" s="2">
-        <v>29.0</v>
+        <v>29</v>
       </c>
       <c r="C46" s="5">
-        <v>45296.0</v>
+        <v>45296</v>
       </c>
       <c r="D46" s="6">
-        <v>0.8333333333333334</v>
-      </c>
-    </row>
-    <row r="47">
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>61</v>
       </c>
       <c r="B47" s="2">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="C47" s="5">
-        <v>45296.0</v>
+        <v>45296</v>
       </c>
       <c r="D47" s="6">
         <v>0.84375</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B48" s="2">
-        <v>42.0</v>
+        <v>42</v>
       </c>
       <c r="C48" s="5">
-        <v>45297.0</v>
+        <v>45297</v>
       </c>
       <c r="D48" s="6">
         <v>0.5</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>67</v>
       </c>
       <c r="B49" s="2">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="C49" s="5">
-        <v>45297.0</v>
+        <v>45297</v>
       </c>
       <c r="D49" s="6">
-        <v>0.5208333333333334</v>
-      </c>
-    </row>
-    <row r="50">
+        <v>0.52083333333333337</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B50" s="2">
-        <v>31.0</v>
+        <v>31</v>
       </c>
       <c r="C50" s="5">
-        <v>45297.0</v>
+        <v>45297</v>
       </c>
       <c r="D50" s="6">
         <v>0.53125</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B51" s="2">
-        <v>22.0</v>
+        <v>22</v>
       </c>
       <c r="C51" s="5">
-        <v>45297.0</v>
+        <v>45297</v>
       </c>
       <c r="D51" s="6">
-        <v>0.5416666666666666</v>
-      </c>
-    </row>
-    <row r="52">
+        <v>0.54166666666666663</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B52" s="2">
-        <v>26.0</v>
+        <v>26</v>
       </c>
       <c r="C52" s="5">
-        <v>45297.0</v>
+        <v>45297</v>
       </c>
       <c r="D52" s="6">
-        <v>0.5520833333333334</v>
-      </c>
-    </row>
-    <row r="53">
+        <v>0.55208333333333337</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B53" s="2">
-        <v>23.0</v>
+        <v>23</v>
       </c>
       <c r="C53" s="5">
-        <v>45297.0</v>
+        <v>45297</v>
       </c>
       <c r="D53" s="6">
         <v>0.75</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B54" s="2">
-        <v>27.0</v>
+        <v>27</v>
       </c>
       <c r="C54" s="5">
-        <v>45297.0</v>
+        <v>45297</v>
       </c>
       <c r="D54" s="6">
-        <v>0.7604166666666666</v>
-      </c>
-    </row>
-    <row r="55">
+        <v>0.76041666666666663</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B55" s="2">
-        <v>38.0</v>
+        <v>38</v>
       </c>
       <c r="C55" s="5">
-        <v>45297.0</v>
+        <v>45297</v>
       </c>
       <c r="D55" s="6">
-        <v>0.7708333333333334</v>
-      </c>
-    </row>
-    <row r="56">
+        <v>0.77083333333333337</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B56" s="2">
-        <v>22.0</v>
+        <v>22</v>
       </c>
       <c r="C56" s="5">
-        <v>45297.0</v>
+        <v>45297</v>
       </c>
       <c r="D56" s="6">
         <v>0.78125</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B57" s="2">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="C57" s="5">
-        <v>45297.0</v>
+        <v>45297</v>
       </c>
       <c r="D57" s="6">
-        <v>0.7916666666666666</v>
-      </c>
-    </row>
-    <row r="58">
+        <v>0.79166666666666663</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B58" s="2">
-        <v>27.0</v>
+        <v>27</v>
       </c>
       <c r="C58" s="5">
-        <v>45297.0</v>
+        <v>45297</v>
       </c>
       <c r="D58" s="6">
-        <v>0.8020833333333334</v>
-      </c>
-    </row>
-    <row r="59">
+        <v>0.80208333333333337</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>61</v>
       </c>
       <c r="B59" s="2">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="C59" s="5">
-        <v>45297.0</v>
+        <v>45297</v>
       </c>
       <c r="D59" s="6">
         <v>0.8125</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B60" s="2">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="C60" s="5">
-        <v>45294.0</v>
+        <v>45294</v>
       </c>
       <c r="D60" s="6">
-        <v>0.7916666666666666</v>
-      </c>
-    </row>
-    <row r="61">
+        <v>0.79166666666666663</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B61" s="2">
-        <v>28.0</v>
+        <v>28</v>
       </c>
       <c r="C61" s="5">
-        <v>45294.0</v>
+        <v>45294</v>
       </c>
       <c r="D61" s="6">
         <v>0.8125</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B62" s="2">
-        <v>28.0</v>
+        <v>28</v>
       </c>
       <c r="C62" s="5">
-        <v>45294.0</v>
+        <v>45294</v>
       </c>
       <c r="D62" s="6">
-        <v>0.8229166666666666</v>
-      </c>
-    </row>
-    <row r="63">
+        <v>0.82291666666666663</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B63" s="2">
-        <v>40.0</v>
+        <v>40</v>
       </c>
       <c r="C63" s="5">
-        <v>45294.0</v>
+        <v>45294</v>
       </c>
       <c r="D63" s="6">
-        <v>0.8333333333333334</v>
-      </c>
-    </row>
-    <row r="64">
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B64" s="2">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="C64" s="5">
-        <v>45294.0</v>
+        <v>45294</v>
       </c>
       <c r="D64" s="6">
         <v>0.84375</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>61</v>
       </c>
       <c r="B65" s="2">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="C65" s="5">
-        <v>45295.0</v>
+        <v>45295</v>
       </c>
       <c r="D65" s="6">
-        <v>0.5208333333333334</v>
-      </c>
-    </row>
-    <row r="66">
+        <v>0.52083333333333337</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B66" s="2">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="C66" s="5">
-        <v>45295.0</v>
+        <v>45295</v>
       </c>
       <c r="D66" s="6">
         <v>0.53125</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B67" s="2">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="C67" s="5">
-        <v>45295.0</v>
+        <v>45295</v>
       </c>
       <c r="D67" s="6">
-        <v>0.5416666666666666</v>
-      </c>
-    </row>
-    <row r="68">
+        <v>0.54166666666666663</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B68" s="2">
-        <v>28.0</v>
+        <v>28</v>
       </c>
       <c r="C68" s="5">
-        <v>45295.0</v>
+        <v>45295</v>
       </c>
       <c r="D68" s="6">
-        <v>0.5520833333333334</v>
-      </c>
-    </row>
-    <row r="69">
+        <v>0.55208333333333337</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B69" s="2">
-        <v>35.0</v>
+        <v>35</v>
       </c>
       <c r="C69" s="5">
-        <v>45295.0</v>
+        <v>45295</v>
       </c>
       <c r="D69" s="6">
-        <v>0.7708333333333334</v>
-      </c>
-    </row>
-    <row r="70">
+        <v>0.77083333333333337</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B70" s="2">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="C70" s="5">
-        <v>45295.0</v>
+        <v>45295</v>
       </c>
       <c r="D70" s="6">
         <v>0.78125</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B71" s="2">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="C71" s="5">
-        <v>45296.0</v>
+        <v>45296</v>
       </c>
       <c r="D71" s="6">
-        <v>0.7916666666666666</v>
-      </c>
-    </row>
-    <row r="72">
+        <v>0.79166666666666663</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B72" s="2">
-        <v>28.0</v>
+        <v>28</v>
       </c>
       <c r="C72" s="5">
-        <v>45296.0</v>
+        <v>45296</v>
       </c>
       <c r="D72" s="6">
-        <v>0.8020833333333334</v>
-      </c>
-    </row>
-    <row r="73">
+        <v>0.80208333333333337</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B73" s="2">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="C73" s="5">
-        <v>45296.0</v>
+        <v>45296</v>
       </c>
       <c r="D73" s="6">
         <v>0.8125</v>
       </c>
     </row>
-    <row r="74">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B74" s="2">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="C74" s="5">
-        <v>45296.0</v>
+        <v>45296</v>
       </c>
       <c r="D74" s="6">
-        <v>0.8229166666666666</v>
-      </c>
-    </row>
-    <row r="75">
+        <v>0.82291666666666663</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B75" s="2">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="C75" s="5">
-        <v>45296.0</v>
+        <v>45296</v>
       </c>
       <c r="D75" s="6">
-        <v>0.8333333333333334</v>
-      </c>
-    </row>
-    <row r="76">
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>61</v>
       </c>
       <c r="B76" s="2">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="C76" s="5">
-        <v>45296.0</v>
+        <v>45296</v>
       </c>
       <c r="D76" s="6">
         <v>0.84375</v>
       </c>
     </row>
-    <row r="77">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B77" s="2">
-        <v>40.0</v>
+        <v>40</v>
       </c>
       <c r="C77" s="5">
-        <v>45297.0</v>
+        <v>45297</v>
       </c>
       <c r="D77" s="6">
         <v>0.5</v>
       </c>
     </row>
-    <row r="78">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>67</v>
       </c>
       <c r="B78" s="2">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="C78" s="5">
-        <v>45297.0</v>
+        <v>45297</v>
       </c>
       <c r="D78" s="6">
-        <v>0.5208333333333334</v>
-      </c>
-    </row>
-    <row r="79">
+        <v>0.52083333333333337</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B79" s="2">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="C79" s="5">
-        <v>45297.0</v>
+        <v>45297</v>
       </c>
       <c r="D79" s="6">
         <v>0.53125</v>
       </c>
     </row>
-    <row r="80">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B80" s="2">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="C80" s="5">
-        <v>45297.0</v>
+        <v>45297</v>
       </c>
       <c r="D80" s="6">
-        <v>0.5416666666666666</v>
-      </c>
-    </row>
-    <row r="81">
+        <v>0.54166666666666663</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B81" s="2">
-        <v>28.0</v>
+        <v>28</v>
       </c>
       <c r="C81" s="5">
-        <v>45297.0</v>
+        <v>45297</v>
       </c>
       <c r="D81" s="6">
-        <v>0.5520833333333334</v>
-      </c>
-    </row>
-    <row r="82">
+        <v>0.55208333333333337</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B82" s="2">
-        <v>28.0</v>
+        <v>28</v>
       </c>
       <c r="C82" s="5">
-        <v>45297.0</v>
+        <v>45297</v>
       </c>
       <c r="D82" s="6">
         <v>0.75</v>
       </c>
     </row>
-    <row r="83">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B83" s="2">
-        <v>28.0</v>
+        <v>28</v>
       </c>
       <c r="C83" s="5">
-        <v>45297.0</v>
+        <v>45297</v>
       </c>
       <c r="D83" s="6">
-        <v>0.7604166666666666</v>
-      </c>
-    </row>
-    <row r="84">
+        <v>0.76041666666666663</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B84" s="2">
-        <v>38.0</v>
+        <v>38</v>
       </c>
       <c r="C84" s="5">
-        <v>45297.0</v>
+        <v>45297</v>
       </c>
       <c r="D84" s="6">
-        <v>0.7708333333333334</v>
-      </c>
-    </row>
-    <row r="85">
+        <v>0.77083333333333337</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B85" s="2">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="C85" s="5">
-        <v>45297.0</v>
+        <v>45297</v>
       </c>
       <c r="D85" s="6">
         <v>0.78125</v>
       </c>
     </row>
-    <row r="86">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B86" s="2">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="C86" s="5">
-        <v>45297.0</v>
+        <v>45297</v>
       </c>
       <c r="D86" s="6">
-        <v>0.7916666666666666</v>
-      </c>
-    </row>
-    <row r="87">
+        <v>0.79166666666666663</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B87" s="2">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="C87" s="5">
-        <v>45297.0</v>
+        <v>45297</v>
       </c>
       <c r="D87" s="6">
-        <v>0.8020833333333334</v>
-      </c>
-    </row>
-    <row r="88">
+        <v>0.80208333333333337</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>61</v>
       </c>
       <c r="B88" s="2">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="C88" s="5">
-        <v>45297.0</v>
+        <v>45297</v>
       </c>
       <c r="D88" s="6">
         <v>0.8125</v>
       </c>
     </row>
-    <row r="89">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B89" s="2">
-        <v>26.0</v>
+        <v>26</v>
       </c>
       <c r="C89" s="5">
-        <v>45297.0</v>
+        <v>45297</v>
       </c>
       <c r="D89" s="6">
-        <v>0.5520833333333334</v>
-      </c>
-    </row>
-    <row r="90">
+        <v>0.55208333333333337</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B90" s="2">
-        <v>23.0</v>
+        <v>23</v>
       </c>
       <c r="C90" s="5">
-        <v>45297.0</v>
+        <v>45297</v>
       </c>
       <c r="D90" s="6">
         <v>0.75</v>
       </c>
     </row>
-    <row r="91">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B91" s="2">
-        <v>27.0</v>
+        <v>27</v>
       </c>
       <c r="C91" s="5">
-        <v>45297.0</v>
+        <v>45297</v>
       </c>
       <c r="D91" s="6">
-        <v>0.7604166666666666</v>
-      </c>
-    </row>
-    <row r="92">
+        <v>0.76041666666666663</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B92" s="2">
-        <v>38.0</v>
+        <v>38</v>
       </c>
       <c r="C92" s="5">
-        <v>45297.0</v>
+        <v>45297</v>
       </c>
       <c r="D92" s="6">
-        <v>0.7708333333333334</v>
-      </c>
-    </row>
-    <row r="93">
+        <v>0.77083333333333337</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B93" s="2">
-        <v>26.0</v>
+        <v>26</v>
       </c>
       <c r="C93" s="5">
-        <v>45297.0</v>
+        <v>45297</v>
       </c>
       <c r="D93" s="6">
-        <v>0.5520833333333334</v>
-      </c>
-    </row>
-    <row r="94">
+        <v>0.55208333333333337</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B94" s="2">
-        <v>23.0</v>
+        <v>23</v>
       </c>
       <c r="C94" s="5">
-        <v>45297.0</v>
+        <v>45297</v>
       </c>
       <c r="D94" s="6">
         <v>0.75</v>
       </c>
     </row>
-    <row r="95">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B95" s="2">
-        <v>27.0</v>
+        <v>27</v>
       </c>
       <c r="C95" s="5">
-        <v>45297.0</v>
+        <v>45297</v>
       </c>
       <c r="D95" s="6">
-        <v>0.7604166666666666</v>
-      </c>
-    </row>
-    <row r="96">
+        <v>0.76041666666666663</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B96" s="2">
-        <v>38.0</v>
+        <v>38</v>
       </c>
       <c r="C96" s="5">
-        <v>45297.0</v>
+        <v>45297</v>
       </c>
       <c r="D96" s="6">
-        <v>0.7708333333333334</v>
-      </c>
-    </row>
-    <row r="97">
+        <v>0.77083333333333337</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B97" s="2">
-        <v>26.0</v>
+        <v>26</v>
       </c>
       <c r="C97" s="5">
-        <v>45297.0</v>
+        <v>45297</v>
       </c>
       <c r="D97" s="6">
-        <v>0.5520833333333334</v>
-      </c>
-    </row>
-    <row r="98">
+        <v>0.55208333333333337</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B98" s="2">
-        <v>23.0</v>
+        <v>23</v>
       </c>
       <c r="C98" s="5">
-        <v>45297.0</v>
+        <v>45297</v>
       </c>
       <c r="D98" s="6">
         <v>0.75</v>
       </c>
     </row>
-    <row r="99">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B99" s="2">
-        <v>27.0</v>
+        <v>27</v>
       </c>
       <c r="C99" s="5">
-        <v>45297.0</v>
+        <v>45297</v>
       </c>
       <c r="D99" s="6">
-        <v>0.7604166666666666</v>
-      </c>
-    </row>
-    <row r="100">
+        <v>0.76041666666666663</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B100" s="2">
-        <v>38.0</v>
+        <v>38</v>
       </c>
       <c r="C100" s="5">
-        <v>45297.0</v>
+        <v>45297</v>
       </c>
       <c r="D100" s="6">
-        <v>0.7708333333333334</v>
-      </c>
-    </row>
-    <row r="101">
+        <v>0.77083333333333337</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B101" s="2">
-        <v>26.0</v>
+        <v>26</v>
       </c>
       <c r="C101" s="5">
-        <v>45297.0</v>
+        <v>45297</v>
       </c>
       <c r="D101" s="6">
-        <v>0.5520833333333334</v>
-      </c>
-    </row>
-    <row r="102">
+        <v>0.55208333333333337</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B102" s="2">
-        <v>23.0</v>
+        <v>23</v>
       </c>
       <c r="C102" s="5">
-        <v>45297.0</v>
+        <v>45297</v>
       </c>
       <c r="D102" s="6">
         <v>0.75</v>
       </c>
     </row>
-    <row r="103">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B103" s="2">
-        <v>27.0</v>
+        <v>27</v>
       </c>
       <c r="C103" s="5">
-        <v>45297.0</v>
+        <v>45297</v>
       </c>
       <c r="D103" s="6">
-        <v>0.7604166666666666</v>
-      </c>
-    </row>
-    <row r="104">
+        <v>0.76041666666666663</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B104" s="2">
-        <v>38.0</v>
+        <v>38</v>
       </c>
       <c r="C104" s="5">
-        <v>45297.0</v>
+        <v>45297</v>
       </c>
       <c r="D104" s="6">
-        <v>0.7708333333333334</v>
-      </c>
-    </row>
-    <row r="105">
+        <v>0.77083333333333337</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B105" s="2">
-        <v>26.0</v>
+        <v>26</v>
       </c>
       <c r="C105" s="5">
-        <v>45297.0</v>
+        <v>45297</v>
       </c>
       <c r="D105" s="6">
-        <v>0.5520833333333334</v>
-      </c>
-    </row>
-    <row r="106">
+        <v>0.55208333333333337</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B106" s="2">
-        <v>23.0</v>
+        <v>23</v>
       </c>
       <c r="C106" s="5">
-        <v>45297.0</v>
+        <v>45297</v>
       </c>
       <c r="D106" s="6">
         <v>0.75</v>
       </c>
     </row>
-    <row r="107">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B107" s="2">
-        <v>27.0</v>
+        <v>27</v>
       </c>
       <c r="C107" s="5">
-        <v>45297.0</v>
+        <v>45297</v>
       </c>
       <c r="D107" s="6">
-        <v>0.7604166666666666</v>
-      </c>
-    </row>
-    <row r="108">
+        <v>0.76041666666666663</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B108" s="2">
-        <v>38.0</v>
+        <v>38</v>
       </c>
       <c r="C108" s="5">
-        <v>45297.0</v>
+        <v>45297</v>
       </c>
       <c r="D108" s="6">
-        <v>0.7708333333333334</v>
-      </c>
-    </row>
-    <row r="109">
+        <v>0.77083333333333337</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B109" s="2">
-        <v>22.0</v>
+        <v>22</v>
       </c>
       <c r="C109" s="5">
-        <v>45294.0</v>
+        <v>45294</v>
       </c>
       <c r="D109" s="6">
         <v>0.84375</v>
       </c>
     </row>
-    <row r="110">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B110" s="2">
-        <v>22.0</v>
+        <v>22</v>
       </c>
       <c r="C110" s="5">
-        <v>45294.0</v>
+        <v>45294</v>
       </c>
       <c r="D110" s="6">
         <v>0.84375</v>
       </c>
     </row>
-    <row r="111">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B111" s="2">
-        <v>22.0</v>
+        <v>22</v>
       </c>
       <c r="C111" s="5">
-        <v>45294.0</v>
+        <v>45294</v>
       </c>
       <c r="D111" s="6">
         <v>0.84375</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>